<commit_message>
- add 2 more channels on coc2 fragment
</commit_message>
<xml_diff>
--- a/app/doc/coclist.xlsx
+++ b/app/doc/coclist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>French</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -152,6 +152,82 @@
   </si>
   <si>
     <t>not work</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UCb87__fTO0TdQcqMBxcNFMQ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Clash Of Clans Vidz | Damien Elledge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>드물게 올라옴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COC Nepal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UCXZ8Ko7yNe9bEMZ8Wri-08A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC5DOhpvPfaUfMdzkQ-9fb5g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clash Of Clans - ClashOnGan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clash of Clans | Eclihpse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UCLAOdac7WmMXQKhOP-8lmrQ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC7Wq4cRGhc1JEF-vr13VsOA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clash Of Clans | GameDiceHD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HaVoC Gaming - Clash of Clans</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC99fa54IUf9RVpEHaUTxQ9w</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clash Of Clans | Mastersaint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_mR72CQd3RVHtmFhlY3O1Q</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clash of Clans with Cam</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UCT2x1vuvgYdhk-kQdlzn6yA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UCaQP9S6tXRHvGOxel7-KFjw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clash of Clans - HDCOC | TeamDTB - Clash of Clans Base Designs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -512,15 +588,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.125" customWidth="1"/>
     <col min="2" max="2" width="28.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -542,166 +618,268 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13">
+        <v>260942</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14">
+        <v>173755</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>87492</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B16" t="s">
         <v>24</v>
       </c>
-      <c r="C13">
+      <c r="C16">
         <v>97364</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17">
+        <v>68647</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18">
+        <v>63041</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19">
+        <v>41647</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20">
+        <v>29701</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21">
+        <v>21074</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>8</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B30" t="s">
         <v>9</v>
       </c>
-      <c r="C17">
+      <c r="C30">
         <v>105289</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>2</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B31" t="s">
         <v>4</v>
       </c>
-      <c r="C18">
+      <c r="C31">
         <v>103753</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>12</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B32" t="s">
         <v>18</v>
       </c>
-      <c r="C19">
+      <c r="C32">
         <v>62392</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>6</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B33" t="s">
         <v>7</v>
       </c>
-      <c r="C20">
+      <c r="C33">
         <v>52539</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>3</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B34" t="s">
         <v>5</v>
       </c>
-      <c r="C21">
+      <c r="C34">
         <v>50775</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>26</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B35" t="s">
         <v>27</v>
       </c>
-      <c r="C22">
+      <c r="C35">
         <v>36126</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>28</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B36" t="s">
         <v>29</v>
       </c>
-      <c r="C23">
+      <c r="C36">
         <v>32692</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>14</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B37" t="s">
         <v>13</v>
       </c>
-      <c r="C24">
+      <c r="C37">
         <v>28901</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>32</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B38" t="s">
         <v>33</v>
       </c>
-      <c r="C25">
+      <c r="C38">
         <v>17938</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>20</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B39" t="s">
         <v>19</v>
       </c>
-      <c r="C26">
+      <c r="C39">
         <v>15714</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>22</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B40" t="s">
         <v>21</v>
       </c>
-      <c r="C27">
+      <c r="C40">
         <v>13170</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>10</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B41" t="s">
         <v>11</v>
       </c>
-      <c r="C28">
+      <c r="C41">
         <v>12857</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>30</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B42" t="s">
         <v>31</v>
       </c>
-      <c r="C29">
+      <c r="C42">
         <v>10919</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- add two more channels on coc2 fragment
</commit_message>
<xml_diff>
--- a/app/doc/coclist.xlsx
+++ b/app/doc/coclist.xlsx
@@ -252,7 +252,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,6 +262,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -280,11 +286,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -591,7 +600,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -741,7 +750,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B30" t="s">
@@ -752,7 +761,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B31" t="s">
@@ -763,7 +772,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B32" t="s">
@@ -774,7 +783,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B33" t="s">

</xml_diff>

<commit_message>
- Material Design is applied - add German CoC channels
</commit_message>
<xml_diff>
--- a/app/doc/coclist.xlsx
+++ b/app/doc/coclist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="89">
   <si>
     <t>French</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -228,6 +228,146 @@
   </si>
   <si>
     <t>Clash of Clans - HDCOC | TeamDTB - Clash of Clans Base Designs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Germany</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLASH OF CLANS COMEDY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UCiTB3QYIaLXhq5UTd_c8EpA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clash of Clans Attacks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC2l8G7UE41Vaby59Dfg6r3w</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Peter17$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UCdtiFB1YxZH_w31YXhsYchQ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clash Of Clans - ClashOnGan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC5DOhpvPfaUfMdzkQ-9fb5g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spencer23$ - Clash Of Clans</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UCKGZr9bU_zuVJPbYdWvIW7g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Daddy - Clash of Clans, join the sidekick army :)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC4GRxPQ7XamQZduBbbinruA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DubWar - Clash &amp; Craft</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UCNsdk80qaH03kBGBP29ZoMA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>need search</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MYSTLC7 - Clash Of Clans</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UCPGnxMlcQtYKLAYymFgB3YA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC4Vxtl8TqjlsPcHzlO7UoIg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UCPJ1htf4qEoAmyoYxVM2brw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DonJon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AretoGaming</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC39FvSwbhLJu0bCxxyUYVqA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elefantenfisch - ClashOfClans und mehr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UCl4-JotWwfpnHaYQp62W23A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lichtle | Clash of Clans</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC6n_2v7YjwZ65F9h77nZPOA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BrennerchenPlays</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UCOwIKNpRYGtb7xso-CdJBRw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tobi Kaiser - QuantumsWeb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UCLEBb3rqJqUqDbky74uuSZA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>in english</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mrmobilefanboy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hatekerr CoC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UCZAGk8POTWog0LBKMDRW99A</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -252,7 +392,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,6 +411,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -286,7 +432,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -294,6 +440,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -597,19 +749,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.125" customWidth="1"/>
-    <col min="2" max="2" width="28.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -620,13 +772,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B13" t="s">
@@ -636,260 +788,453 @@
         <v>260942</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14">
+        <v>233086</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>47</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>173755</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>41</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>40</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>87492</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16">
-        <v>97364</v>
-      </c>
-      <c r="D16" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C17">
-        <v>68647</v>
+        <v>97364</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C18">
-        <v>63041</v>
+        <v>68647</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C19">
-        <v>41647</v>
+        <v>63041</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C20">
-        <v>29701</v>
+        <v>41647</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C21">
-        <v>21074</v>
+        <v>29701</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22">
+        <v>21074</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>38</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>39</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <v>4579</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24">
+        <v>287825</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25">
+        <v>486977</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26">
+        <v>26934</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27">
+        <v>88529</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28">
+        <v>12099</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29">
+        <v>67341</v>
+      </c>
+      <c r="D29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30">
+        <v>142257</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B36" t="s">
         <v>9</v>
       </c>
-      <c r="C30">
+      <c r="C36">
         <v>105289</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B37" t="s">
         <v>4</v>
       </c>
-      <c r="C31">
+      <c r="C37">
         <v>103753</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B38" t="s">
         <v>18</v>
       </c>
-      <c r="C32">
+      <c r="C38">
         <v>62392</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B39" t="s">
         <v>7</v>
       </c>
-      <c r="C33">
+      <c r="C39">
         <v>52539</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34">
-        <v>50775</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" t="s">
-        <v>27</v>
-      </c>
-      <c r="C35">
-        <v>36126</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>28</v>
-      </c>
-      <c r="B36" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36">
-        <v>32692</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37">
-        <v>28901</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38">
-        <v>17938</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>20</v>
-      </c>
-      <c r="B39" t="s">
-        <v>19</v>
-      </c>
-      <c r="C39">
-        <v>15714</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C40">
-        <v>13170</v>
+        <v>50775</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B41" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C41">
-        <v>12857</v>
+        <v>36126</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42">
+        <v>32692</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43">
+        <v>28901</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44">
+        <v>17938</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45">
+        <v>15714</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46">
+        <v>13170</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47">
+        <v>12857</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>30</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B48" t="s">
         <v>31</v>
       </c>
-      <c r="C42">
+      <c r="C48">
         <v>10919</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51">
+        <v>177966</v>
+      </c>
+      <c r="D51" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B52" t="s">
+        <v>73</v>
+      </c>
+      <c r="C52">
+        <v>150516</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B53" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53">
+        <v>106786</v>
+      </c>
+      <c r="D53" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>81</v>
+      </c>
+      <c r="B54" t="s">
+        <v>82</v>
+      </c>
+      <c r="C54">
+        <v>32413</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C55">
+        <v>17777</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>75</v>
+      </c>
+      <c r="B56" t="s">
+        <v>76</v>
+      </c>
+      <c r="C56">
+        <v>8127</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57" t="s">
+        <v>78</v>
+      </c>
+      <c r="C57">
+        <v>3536</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>79</v>
+      </c>
+      <c r="B58" t="s">
+        <v>80</v>
+      </c>
+      <c r="C58">
+        <v>7363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- add SWC clans channel
</commit_message>
<xml_diff>
--- a/app/doc/coclist.xlsx
+++ b/app/doc/coclist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
   <si>
     <t>French</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -368,6 +368,18 @@
   </si>
   <si>
     <t>UCZAGk8POTWog0LBKMDRW99A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC_lPhq9a6rG76HXRFCl0zAw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SWC Clan Wars</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한달후 확인</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -432,7 +444,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -446,6 +458,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -751,14 +766,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.125" customWidth="1"/>
     <col min="2" max="2" width="32.875" customWidth="1"/>
+    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -982,6 +998,20 @@
       </c>
       <c r="C30">
         <v>142257</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="5">
+        <v>42124</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>